<commit_message>
Fixed up energy spreadsheets
</commit_message>
<xml_diff>
--- a/maps/AZ/AZ20C_energies.xlsx
+++ b/maps/AZ/AZ20C_energies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alecramsay/Documents/dev/baseline/maps/AZ/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{273C5632-5AF3-F14C-B533-C3AD1E875537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A73E9E8-B747-5D48-89BC-B14E3A407763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="560" windowWidth="27640" windowHeight="17440" activeTab="1" xr2:uid="{95FC3DAC-F24A-7C41-AFDA-0418D017069F}"/>
+    <workbookView xWindow="1420" yWindow="560" windowWidth="27640" windowHeight="17440" xr2:uid="{95FC3DAC-F24A-7C41-AFDA-0418D017069F}"/>
   </bookViews>
   <sheets>
     <sheet name="SUMMARY" sheetId="2" r:id="rId1"/>
@@ -877,8 +877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F745D026-6BA9-AB45-93E7-0E1B1C1D9B8C}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -914,19 +914,19 @@
         <v>83</v>
       </c>
       <c r="B4" s="7">
-        <f>MIN(DATA!E$2:E$126)</f>
+        <f>MIN(DATA!E$2:E$101)</f>
         <v>0</v>
       </c>
       <c r="C4" s="7">
-        <f>MIN(DATA!F$2:F$126)</f>
+        <f>MIN(DATA!F$2:F$101)</f>
         <v>0.75765099999999996</v>
       </c>
       <c r="D4" s="7">
-        <f>MIN(DATA!G$2:G$126)</f>
+        <f>MIN(DATA!G$2:G$101)</f>
         <v>0</v>
       </c>
       <c r="E4" s="7">
-        <f>MIN(DATA!H$2:H$126)</f>
+        <f>MIN(DATA!H$2:H$101)</f>
         <v>0</v>
       </c>
     </row>
@@ -935,19 +935,19 @@
         <v>84</v>
       </c>
       <c r="B5" s="7">
-        <f>MAX(DATA!E$2:E$126)</f>
+        <f>MAX(DATA!E$2:E$101)</f>
         <v>2.6046E-2</v>
       </c>
       <c r="C5" s="7">
-        <f>MAX(DATA!F$2:F$126)</f>
+        <f>MAX(DATA!F$2:F$101)</f>
         <v>1</v>
       </c>
       <c r="D5" s="7">
-        <f>MAX(DATA!G$2:G$126)</f>
+        <f>MAX(DATA!G$2:G$101)</f>
         <v>0.84905799999999998</v>
       </c>
       <c r="E5" s="7">
-        <f>MAX(DATA!H$2:H$126)</f>
+        <f>MAX(DATA!H$2:H$101)</f>
         <v>0.66247299999999998</v>
       </c>
     </row>
@@ -956,19 +956,19 @@
         <v>85</v>
       </c>
       <c r="B6" s="7">
-        <f>AVERAGE(DATA!E$2:E$126)</f>
+        <f>AVERAGE(DATA!E$2:E$101)</f>
         <v>7.6533367346938797E-3</v>
       </c>
       <c r="C6" s="7">
-        <f>AVERAGE(DATA!F$2:F$126)</f>
+        <f>AVERAGE(DATA!F$2:F$101)</f>
         <v>0.90478279591836819</v>
       </c>
       <c r="D6" s="7">
-        <f>AVERAGE(DATA!G$2:G$126)</f>
+        <f>AVERAGE(DATA!G$2:G$101)</f>
         <v>0.37239824489795886</v>
       </c>
       <c r="E6" s="7">
-        <f>AVERAGE(DATA!H$2:H$126)</f>
+        <f>AVERAGE(DATA!H$2:H$101)</f>
         <v>0.23270855102040808</v>
       </c>
     </row>
@@ -977,19 +977,19 @@
         <v>86</v>
       </c>
       <c r="B7" s="7">
-        <f>MEDIAN(DATA!E$2:E$126)</f>
+        <f>MEDIAN(DATA!E$2:E$101)</f>
         <v>7.8385E-3</v>
       </c>
       <c r="C7" s="7">
-        <f>MEDIAN(DATA!F$2:F$126)</f>
+        <f>MEDIAN(DATA!F$2:F$101)</f>
         <v>0.94670200000000004</v>
       </c>
       <c r="D7" s="7">
-        <f>MEDIAN(DATA!G$2:G$126)</f>
+        <f>MEDIAN(DATA!G$2:G$101)</f>
         <v>0.32064100000000001</v>
       </c>
       <c r="E7" s="7">
-        <f>MEDIAN(DATA!H$2:H$126)</f>
+        <f>MEDIAN(DATA!H$2:H$101)</f>
         <v>0.11714050000000001</v>
       </c>
     </row>
@@ -998,19 +998,19 @@
         <v>87</v>
       </c>
       <c r="B8" s="10">
-        <f>STDEV(DATA!E$2:E$126)</f>
+        <f>STDEV(DATA!E$2:E$101)</f>
         <v>3.6297753784238357E-3</v>
       </c>
       <c r="C8" s="10">
-        <f>STDEV(DATA!F$2:F$126)</f>
+        <f>STDEV(DATA!F$2:F$101)</f>
         <v>8.0893739246352597E-2</v>
       </c>
       <c r="D8" s="10">
-        <f>STDEV(DATA!G$2:G$126)</f>
+        <f>STDEV(DATA!G$2:G$101)</f>
         <v>0.2255393438653619</v>
       </c>
       <c r="E8" s="10">
-        <f>STDEV(DATA!H$2:H$126)</f>
+        <f>STDEV(DATA!H$2:H$101)</f>
         <v>0.2089343561575048</v>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
         <v>91</v>
       </c>
       <c r="D13" s="13">
-        <f>COUNTIF(DATA!E2:E126, "&lt;0.01")</f>
+        <f>COUNTIF(DATA!E2:E101, "&lt;0.01")</f>
         <v>87</v>
       </c>
       <c r="E13" s="17">
@@ -1071,7 +1071,7 @@
         <v>92</v>
       </c>
       <c r="D14" s="13">
-        <f>COUNTIF(DATA!F2:F126, "&gt;0.95")</f>
+        <f>COUNTIF(DATA!F2:F101, "&gt;0.95")</f>
         <v>36</v>
       </c>
       <c r="E14" s="17">
@@ -1084,7 +1084,7 @@
         <v>97</v>
       </c>
       <c r="D15">
-        <f>COUNTIF(DATA!C2:C126, FALSE)</f>
+        <f>COUNTIF(DATA!C2:C101, FALSE)</f>
         <v>1</v>
       </c>
       <c r="E15" s="17">
@@ -1101,7 +1101,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5CE2F69-B1C4-F145-9310-B57BB43ED826}">
   <dimension ref="A1:I99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>